<commit_message>
commit changes to main for feature files
</commit_message>
<xml_diff>
--- a/src/main/resources/FeatureFiles/ContactUsPage_Chrome.xlsx
+++ b/src/main/resources/FeatureFiles/ContactUsPage_Chrome.xlsx
@@ -294,7 +294,7 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>openBrowser</t>
+    <t>openHeadlessBrowser</t>
   </si>
 </sst>
 </file>
@@ -697,7 +697,7 @@
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>92</v>
       </c>
       <c r="D2" s="2" t="s">

</xml_diff>